<commit_message>
Added a sheet to the check genotypes spreadsheet to hold just the yield checks, and not the yield checks and the parents. Also added a script to the sandbox folder where I was messing around with the custom contrasts in emmeans
</commit_message>
<xml_diff>
--- a/data/utils/check_genotypes.xlsx
+++ b/data/utils/check_genotypes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\R\Projects\Jay_yield\data\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhgille2\Documents\R\projects\Jay_yield\data\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76955A50-5201-465D-AC12-C9EF81D0AD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F426DF-DA86-460B-BF34-61758D2987AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9430" yWindow="3660" windowWidth="14620" windowHeight="11770" xr2:uid="{6FADE5DA-DF96-4F75-B103-F4D8E9C97C40}"/>
+    <workbookView xWindow="-67530" yWindow="2085" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{6FADE5DA-DF96-4F75-B103-F4D8E9C97C40}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checks_and_parents" sheetId="1" r:id="rId1"/>
+    <sheet name="yield_checks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>genotype</t>
   </si>
@@ -433,84 +434,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC25BC7-722A-415D-BF17-E871AF892CCD}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180FB505-358A-4CEC-8F46-B0B5FFDD7729}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>